<commit_message>
guowei  -- 验证码的domain 不对
</commit_message>
<xml_diff>
--- a/www/web/other/kf_word_20200203.xlsx
+++ b/www/web/other/kf_word_20200203.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/code/guangzhou/kefu/www/web/other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9A51E7-E863-FE48-B695-36CA2B0F307C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382E38E7-B178-7A47-8DAF-951273E89C59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27940" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="2200" windowWidth="27940" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -363,13 +363,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" style="1"/>
+    <col min="1" max="1" width="15.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="99.33203125" style="1" customWidth="1"/>
     <col min="3" max="16384" width="18.83203125" style="1"/>
   </cols>

</xml_diff>